<commit_message>
Formatting performed to highlight the required elements
</commit_message>
<xml_diff>
--- a/cloud_scheduling_downtime.xlsx
+++ b/cloud_scheduling_downtime.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\KE5207-FM-GA\CI2_GA_code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FCEE161E-4674-4169-B6AA-AB437BC80D02}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{22320C79-208D-412E-8E28-7339E26E20FE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="23535" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -163,7 +163,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Anurag Chatterjee:</t>
         </r>
@@ -172,7 +172,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Calculated by dividing by efficiency</t>
@@ -187,7 +187,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Anurag Chatterjee:</t>
         </r>
@@ -196,7 +196,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 After pre-emtion # jobs the machine is unavailable for pre emption time and so it adds to the time</t>
@@ -368,17 +368,17 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -398,6 +398,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -585,7 +591,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
@@ -610,6 +616,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Calculation" xfId="3" builtinId="22"/>
@@ -1068,7 +1075,7 @@
   <dimension ref="A1:W17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1154,10 +1161,10 @@
       <c r="J2" s="16">
         <v>0</v>
       </c>
-      <c r="K2" s="17">
-        <v>0</v>
-      </c>
-      <c r="L2">
+      <c r="K2" s="16">
+        <v>0</v>
+      </c>
+      <c r="L2" s="17">
         <v>0</v>
       </c>
       <c r="M2">
@@ -1205,10 +1212,10 @@
       <c r="J3" s="19">
         <v>1</v>
       </c>
-      <c r="K3" s="20">
-        <v>1</v>
-      </c>
-      <c r="L3">
+      <c r="K3" s="19">
+        <v>1</v>
+      </c>
+      <c r="L3" s="20">
         <v>0</v>
       </c>
       <c r="M3">
@@ -1256,10 +1263,10 @@
       <c r="J4" s="22">
         <v>0</v>
       </c>
-      <c r="K4" s="23">
-        <v>0</v>
-      </c>
-      <c r="L4">
+      <c r="K4" s="22">
+        <v>0</v>
+      </c>
+      <c r="L4" s="23">
         <v>1</v>
       </c>
       <c r="M4">
@@ -1281,47 +1288,47 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C5">
-        <f>SUM(C2:C4)</f>
+        <f t="shared" ref="C5:M5" si="0">SUM(C2:C4)</f>
         <v>1</v>
       </c>
       <c r="D5">
-        <f>SUM(D2:D4)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E5">
-        <f>SUM(E2:E4)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F5">
-        <f>SUM(F2:F4)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G5">
-        <f>SUM(G2:G4)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H5">
-        <f>SUM(H2:H4)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I5">
-        <f>SUM(I2:I4)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J5">
-        <f>SUM(J2:J4)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K5">
-        <f>SUM(K2:K4)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L5">
-        <f>SUM(L2:L4)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="M5">
-        <f>SUM(M2:M4)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
@@ -1338,7 +1345,7 @@
       <c r="O7" t="s">
         <v>30</v>
       </c>
-      <c r="P7">
+      <c r="P7" s="24">
         <f>SUM(O2:O4)+INT(M2/W13)*V13+INT(M3/W14)*V14+INT(M4/W15)*V15</f>
         <v>6.9083333333333332</v>
       </c>

</xml_diff>